<commit_message>
Recovery Category in resources
</commit_message>
<xml_diff>
--- a/Game Design/ResourceList.xlsx
+++ b/Game Design/ResourceList.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allan\Documents\GitHub\BeforeLegends\Game Design\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
@@ -15,11 +10,11 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$K$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$L$37</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="55">
   <si>
     <t>Mountains</t>
   </si>
@@ -189,13 +184,16 @@
   </si>
   <si>
     <t>Wild Lentil</t>
+  </si>
+  <si>
+    <t>Recovery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,6 +264,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -389,7 +393,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -404,6 +408,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="2" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Ausgabe" xfId="4" builtinId="21"/>
@@ -469,7 +474,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -504,7 +509,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -681,36 +686,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="62.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1">
       <c r="A1" s="5" t="s">
         <v>38</v>
       </c>
@@ -723,29 +729,32 @@
       <c r="D1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -754,12 +763,10 @@
         <v>37</v>
       </c>
       <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="G2" s="3" t="s">
         <v>37</v>
       </c>
@@ -772,9 +779,12 @@
       <c r="J2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -785,23 +795,24 @@
         <v>37</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="I3" s="4"/>
       <c r="J3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -812,21 +823,22 @@
         <v>37</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="I4" s="4"/>
       <c r="J4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -837,23 +849,24 @@
         <v>37</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="4"/>
       <c r="G5" s="4"/>
-      <c r="H5" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -866,25 +879,26 @@
       <c r="D6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="G6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
         <v>37</v>
       </c>
       <c r="J6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -895,17 +909,18 @@
         <v>37</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -918,17 +933,18 @@
       <c r="D8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="4"/>
+      <c r="F8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -939,17 +955,18 @@
         <v>37</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
@@ -960,17 +977,18 @@
         <v>37</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -983,17 +1001,18 @@
       <c r="D11" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="4"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1006,17 +1025,18 @@
       <c r="D12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -1027,17 +1047,18 @@
       <c r="D13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
@@ -1048,17 +1069,18 @@
       <c r="D14" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1069,17 +1091,18 @@
       <c r="D15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="4"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="1" t="s">
         <v>19</v>
       </c>
@@ -1090,23 +1113,24 @@
       <c r="D16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="H16" s="4"/>
-      <c r="I16" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="I16" s="4"/>
       <c r="J16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1117,23 +1141,24 @@
       <c r="D17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="4"/>
+      <c r="G17" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="H17" s="4"/>
-      <c r="I17" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="I17" s="4"/>
       <c r="J17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
@@ -1144,17 +1169,18 @@
       <c r="D18" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
@@ -1165,12 +1191,10 @@
         <v>37</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="G19" s="4" t="s">
         <v>37</v>
       </c>
@@ -1184,10 +1208,13 @@
         <v>37</v>
       </c>
       <c r="K19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -1200,19 +1227,20 @@
       <c r="D20" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="4" t="s">
+      <c r="K20" s="4"/>
+      <c r="L20" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
         <v>32</v>
       </c>
@@ -1225,19 +1253,20 @@
       <c r="D21" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="4" t="s">
+      <c r="K21" s="4"/>
+      <c r="L21" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="1" t="s">
         <v>33</v>
       </c>
@@ -1250,19 +1279,20 @@
       <c r="D22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="4" t="s">
+      <c r="K22" s="4"/>
+      <c r="L22" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -1275,17 +1305,18 @@
       <c r="D23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
@@ -1296,17 +1327,18 @@
       <c r="D24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="1" t="s">
         <v>46</v>
       </c>
@@ -1317,17 +1349,18 @@
       <c r="D25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="4"/>
+      <c r="F25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -1338,21 +1371,22 @@
       <c r="D26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="4"/>
+      <c r="F26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="I26" s="4"/>
       <c r="J26" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
@@ -1363,25 +1397,26 @@
       <c r="D27" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="4"/>
+      <c r="F27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G27" s="4"/>
+      <c r="G27" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="H27" s="4"/>
-      <c r="I27" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="I27" s="4"/>
       <c r="J27" s="4" t="s">
         <v>37</v>
       </c>
       <c r="K27" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L27" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -1392,21 +1427,22 @@
         <v>37</v>
       </c>
       <c r="D28" s="4"/>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="4"/>
+      <c r="F28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="I28" s="4"/>
       <c r="J28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="1:12">
       <c r="A29" s="1" t="s">
         <v>51</v>
       </c>
@@ -1417,17 +1453,18 @@
         <v>37</v>
       </c>
       <c r="D29" s="4"/>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="4"/>
+      <c r="F29" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="4"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="1:12">
       <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
@@ -1438,21 +1475,22 @@
         <v>37</v>
       </c>
       <c r="D30" s="4"/>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="4"/>
+      <c r="F30" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
-      <c r="I30" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="I30" s="4"/>
       <c r="J30" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="1:12">
       <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
@@ -1463,21 +1501,22 @@
         <v>37</v>
       </c>
       <c r="D31" s="4"/>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="4"/>
+      <c r="F31" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
-      <c r="I31" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="I31" s="4"/>
       <c r="J31" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="K31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="1:12">
       <c r="A32" s="1"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1489,8 +1528,9 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="1:12">
       <c r="A33" s="1"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1502,8 +1542,9 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="1:12">
       <c r="A34" s="1"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1515,8 +1556,9 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="1:12">
       <c r="A35" s="1"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1528,8 +1570,9 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="4"/>
+    </row>
+    <row r="36" spans="1:12">
       <c r="A36" s="1"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1541,8 +1584,9 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="1:12">
       <c r="A37" s="1"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1554,9 +1598,12 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K37"/>
+  <autoFilter ref="A1:L37">
+    <filterColumn colId="4"/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>